<commit_message>
EDA complete. Single function solution
</commit_message>
<xml_diff>
--- a/CH-156 Column Splitting.xlsx
+++ b/CH-156 Column Splitting.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521F55EC-458E-4461-8FBA-D0975BA8376F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1773709F-562E-4E91-833C-A55DEA6F696E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$14</definedName>
+    <definedName name="fc">_xlfn.LAMBDA(_xlpm.t,IFERROR(_xlpm.t+0,_xlpm.t))</definedName>
+    <definedName name="fn">_xlfn.LAMBDA(_xlpm.s, _xlfn.LET( _xlpm.l,LEN(_xlpm.s), _xlpm.ev,fc(_xlfn.HSTACK(LEFT(_xlpm.s,_xlpm.l/2),RIGHT(_xlpm.s,_xlpm.l/2),"")), _xlpm.od,_xlfn.HSTACK(LEFT(_xlpm.s,FLOOR(_xlpm.l/2,1)),MID(_xlpm.s,FLOOR(_xlpm.l/2,1)+1,1),RIGHT(_xlpm.s,_xlpm.l-CEILING(_xlpm.l/2,1))),IF(MOD(_xlpm.l,2),_xlpm.od,_xlpm.ev)) )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +42,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Question</t>
   </si>
@@ -108,6 +134,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
+  </si>
+  <si>
+    <t>RS</t>
   </si>
 </sst>
 </file>
@@ -807,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1000,4 +1029,341 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D18E03-8BAF-4C26-9328-F5DDBBFEDD86}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="54" customWidth="1"/>
+    <col min="4" max="4" width="8.69921875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="8.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="I1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="14">
+        <v>12</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>28</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="b">
+        <f>ISNUMBER(F4)</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8" t="b">
+        <f>ISNUMBER(E6)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="G10" cm="1">
+        <f t="array" ref="G10">_xlfn.LAMBDA(_xlpm.t,IFERROR(_xlpm.t+0,_xlpm.t))("12")</f>
+        <v>12</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="str" cm="1">
+        <f t="array" ref="C12:E12">_xlfn.LAMBDA(_xlpm.s,
+_xlfn.LET(
+_xlpm.l,LEN(_xlpm.s),
+_xlpm.ev,fc(_xlfn.HSTACK(LEFT(_xlpm.s,_xlpm.l/2),RIGHT(_xlpm.s,_xlpm.l/2),"")),
+_xlpm.od,_xlfn.HSTACK(LEFT(_xlpm.s,FLOOR(_xlpm.l/2,1)),MID(_xlpm.s,FLOOR(_xlpm.l/2,1)+1,1),RIGHT(_xlpm.s,_xlpm.l-CEILING(_xlpm.l/2,1))),IF(MOD(_xlpm.l,2),_xlpm.od,_xlpm.ev))
+)("HiMark")</f>
+        <v>HiM</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <v>ark</v>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="str" cm="1">
+        <f t="array" ref="C14:E19">_xlfn.DROP(_xlfn.REDUCE("",B3:B8,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,fn(_xlpm.v)))),1)</f>
+        <v>MN</v>
+      </c>
+      <c r="D14" s="5">
+        <v>12</v>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="G14" t="b" cm="1">
+        <f t="array" ref="G14:I19">_xlfn.ANCHORARRAY(C14)=D3:F8</f>
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="str">
+        <v>MX</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <v>28</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16" t="str">
+        <v>RS</v>
+      </c>
+      <c r="D16" s="5" t="str">
+        <v>M</v>
+      </c>
+      <c r="E16" t="str">
+        <v>55</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" t="str">
+        <v>FFm</v>
+      </c>
+      <c r="D17" s="5">
+        <v>210</v>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" t="str">
+        <v>S</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="E18" t="str">
+        <v>2</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="str">
+        <v>S</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <v>S</v>
+      </c>
+      <c r="E19" t="str">
+        <v>S</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Analysis of second ALT
</commit_message>
<xml_diff>
--- a/CH-156 Column Splitting.xlsx
+++ b/CH-156 Column Splitting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098C0F1D-868F-4B7E-8EAD-07A925BE61EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E77833E-3D0B-4DFE-92DD-72870BDDCADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
   <si>
     <t>Question</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Mark</t>
+  </si>
+  <si>
+    <t>This is the best thing I learned here. I can insert by not stating the number of characters to replace.</t>
   </si>
 </sst>
 </file>
@@ -857,6 +860,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1712,7 +1718,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D16"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1873,6 +1879,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
+      <c r="H10" t="str">
+        <f>REPLACE("1234567", 7/2 + 1, , "|")</f>
+        <v>123|4567</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>